<commit_message>
pay salary added with date
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Employee.xlsx
+++ b/src/main/resources/data/Employee.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="report-sheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="employee-sheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'report-sheet'!$B$1:$B$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'employee-sheet'!$B$1:$B$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -136,7 +136,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,6 +157,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,17 +199,17 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="986" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="13.23" collapsed="false" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="16.31" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="21.49" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="20.17" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="false" hidden="false" style="1" width="8.54" collapsed="false" outlineLevel="0"/>
+    <col min="986" max="1024" customWidth="true" hidden="false" style="0" width="9.14" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,7 +237,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>44846.1474884259</v>
+        <v>44865.973287037</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -248,15 +249,15 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>148.5</v>
+        <v>3000.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>44866.1474884259</v>
+      <c r="B3" s="5" t="n">
+        <v>44884.986863645834</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>9</v>
@@ -268,7 +269,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0</v>
+        <v>40000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>